<commit_message>
updated passage and word list
</commit_message>
<xml_diff>
--- a/passages.xlsx
+++ b/passages.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajnafannikertesz/Desktop/Accents /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316AE168-23C3-5346-A37F-65A87509661E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE88E23-BCDD-8049-970E-70E1D0307B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="10660" windowHeight="15600" xr2:uid="{B4675F82-FACE-3948-ABD8-6695BD5CDA27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
   <si>
     <t>target</t>
   </si>
@@ -50,13 +50,7 @@
     <t>ants</t>
   </si>
   <si>
-    <t>romans</t>
-  </si>
-  <si>
     <t>otzi</t>
-  </si>
-  <si>
-    <t>kocs</t>
   </si>
   <si>
     <t>US</t>
@@ -420,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDCEFFC-7E2A-4A4D-95AF-8BA28921EB86}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,7 +430,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -444,7 +438,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT("passages/NewZealand_",A2,".wav")</f>
@@ -456,10 +450,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C7" si="0">_xlfn.CONCAT("passages/NewZealand_",A3,".wav")</f>
+        <f t="shared" ref="C3:C4" si="0">_xlfn.CONCAT("passages/NewZealand_",A3,".wav")</f>
         <v>passages/NewZealand_ants.wav</v>
       </c>
     </row>
@@ -468,155 +462,83 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>passages/NewZealand_romans.wav</v>
+        <v>passages/NewZealand_otzi.wav</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>passages/NewZealand_otzi.wav</v>
+        <f>_xlfn.CONCAT("passages/American_",A5,".wav")</f>
+        <v>passages/American_coffee.wav</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>passages/NewZealand_kocs.wav</v>
+        <f t="shared" ref="C6:C7" si="1">_xlfn.CONCAT("passages/American_",A6,".wav")</f>
+        <v>passages/American_ants.wav</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" t="str">
-        <f>_xlfn.CONCAT("passages/American_",A7,".wav")</f>
-        <v>passages/American_coffee.wav</v>
+        <f t="shared" si="1"/>
+        <v>passages/American_otzi.wav</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" ref="C8:C12" si="1">_xlfn.CONCAT("passages/American_",A8,".wav")</f>
-        <v>passages/American_ants.wav</v>
+        <f>_xlfn.CONCAT("passages/Turkish_",A8,".wav")</f>
+        <v>passages/Turkish_coffee.wav</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="1"/>
-        <v>passages/American_romans.wav</v>
+        <f t="shared" ref="C9:C10" si="2">_xlfn.CONCAT("passages/Turkish_",A9,".wav")</f>
+        <v>passages/Turkish_ants.wav</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" si="1"/>
-        <v>passages/American_otzi.wav</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="1"/>
-        <v>passages/American_kocs.wav</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="str">
-        <f>_xlfn.CONCAT("passages/Turkish_",A12,".wav")</f>
-        <v>passages/Turkish_coffee.wav</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" ref="C13:C16" si="2">_xlfn.CONCAT("passages/Turkish_",A13,".wav")</f>
-        <v>passages/Turkish_ants.wav</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="2"/>
-        <v>passages/Turkish_romans.wav</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="str">
         <f t="shared" si="2"/>
         <v>passages/Turkish_otzi.wav</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="2"/>
-        <v>passages/Turkish_kocs.wav</v>
       </c>
     </row>
   </sheetData>

</xml_diff>